<commit_message>
added another input mode
</commit_message>
<xml_diff>
--- a/CollegeCalculator/Colleges.xlsx
+++ b/CollegeCalculator/Colleges.xlsx
@@ -434,7 +434,7 @@
         <v>0.4</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3719372458539626</v>
+        <v>0.9816078898292088</v>
       </c>
       <c r="G2" t="n">
         <v>0.4</v>
@@ -462,7 +462,7 @@
         <v>0.4</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3051210871649344</v>
+        <v>0.3093259448199278</v>
       </c>
       <c r="G3" t="n">
         <v>0.4</v>
@@ -490,7 +490,7 @@
         <v>0.4</v>
       </c>
       <c r="F4" t="n">
-        <v>0.5496586720801736</v>
+        <v>0.528011429751901</v>
       </c>
       <c r="G4" t="n">
         <v>0.4</v>
@@ -518,7 +518,7 @@
         <v>0.4</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2038211866759204</v>
+        <v>0.2211431802606283</v>
       </c>
       <c r="G5" t="n">
         <v>0.4</v>
@@ -546,7 +546,7 @@
         <v>0.4</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9560788436221284</v>
+        <v>0.2025396008973027</v>
       </c>
       <c r="G6" t="n">
         <v>0.4</v>
@@ -574,7 +574,7 @@
         <v>0.4</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4315214011952644</v>
+        <v>0.3353222317810357</v>
       </c>
       <c r="G7" t="n">
         <v>0.4</v>
@@ -602,7 +602,7 @@
         <v>0.4</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5459010644997834</v>
+        <v>0.480881821685384</v>
       </c>
       <c r="G8" t="n">
         <v>0.4</v>
@@ -630,7 +630,7 @@
         <v>0.4</v>
       </c>
       <c r="F9" t="n">
-        <v>0.2434439633367786</v>
+        <v>0.2456892014419062</v>
       </c>
       <c r="G9" t="n">
         <v>0.4</v>
@@ -658,7 +658,7 @@
         <v>0.4</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2169003406940172</v>
+        <v>0.6399064000863915</v>
       </c>
       <c r="G10" t="n">
         <v>0.4</v>
@@ -686,7 +686,7 @@
         <v>0.4</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2153690716396996</v>
+        <v>0.3897293990344669</v>
       </c>
       <c r="G11" t="n">
         <v>0.4</v>
@@ -714,7 +714,7 @@
         <v>0.4</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4331583276262417</v>
+        <v>0.4177155948873165</v>
       </c>
       <c r="G12" t="n">
         <v>0.4</v>
@@ -742,7 +742,7 @@
         <v>0.4</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3134170039045866</v>
+        <v>0.3291603309168202</v>
       </c>
       <c r="G13" t="n">
         <v>0.4</v>
@@ -770,7 +770,7 @@
         <v>0.4</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2441967251770852</v>
+        <v>0.2592286777889876</v>
       </c>
       <c r="G14" t="n">
         <v>0.4</v>
@@ -798,7 +798,7 @@
         <v>0.4</v>
       </c>
       <c r="F15" t="n">
-        <v>0.3938136972382493</v>
+        <v>0.2509383021706575</v>
       </c>
       <c r="G15" t="n">
         <v>0.4</v>
@@ -826,7 +826,7 @@
         <v>0.4</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2694258064129177</v>
+        <v>0.2636604920511952</v>
       </c>
       <c r="G16" t="n">
         <v>0.4</v>
@@ -854,7 +854,7 @@
         <v>0.4</v>
       </c>
       <c r="F17" t="n">
-        <v>0.8472451947293224</v>
+        <v>0.7188558658383181</v>
       </c>
       <c r="G17" t="n">
         <v>0.4</v>
@@ -882,7 +882,7 @@
         <v>0.4</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5323244651821591</v>
+        <v>0.2305833645066783</v>
       </c>
       <c r="G18" t="n">
         <v>0.4</v>

</xml_diff>